<commit_message>
Updated to modern openpyxl functions
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,14 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlake\git\learning_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D8294C-C434-4C69-84F5-FA992BB3FDAF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDEA406C-86CF-4896-8C47-0EDBD60DA739}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="3075" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{15B35DD3-46EC-4C7B-8B11-6A72A1C60266}"/>
+    <workbookView xWindow="6075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{15B35DD3-46EC-4C7B-8B11-6A72A1C60266}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
   <si>
     <t>ip_address</t>
   </si>
@@ -123,9 +121,6 @@
   </si>
   <si>
     <t>Extranet</t>
-  </si>
-  <si>
-    <t>test</t>
   </si>
 </sst>
 </file>
@@ -485,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5357593C-174C-47A0-8A19-E7FF2D67DE65}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,42 +862,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED4DEB9-C64B-4E5F-99F8-B47B71AE41E1}">
-  <dimension ref="B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36C462A7-7CDD-4139-9D4B-CFA78CE863FC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>